<commit_message>
Refactor log files and update gitignore
</commit_message>
<xml_diff>
--- a/log/nli_model_log.xlsx
+++ b/log/nli_model_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,6 +455,1526 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>C'nin dikkat ve özen yükümlülüğüne aykırı davranmış olması nedeniyle kusurlu olduğu değerlendirilebilir.</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>C'nin dikkat ve özen yükümlülüğüne aykırı davranmış olması nedeniyle kusurlu olduğu değerlendrilemez.</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>ENTAILMENT</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.7691475749015808</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>C'nin dikkat ve özen yükümlülüğüne aykırı davranmış olması nedeniyle kusurlu olduğu değerlendirilebilir.</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>C kişisi marketten alışveriş yapmıştır ve kasada ödeme yapmadan çıkmıştır.</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.5896795392036438</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>C'nin dikkat ve özen yükümlülüğüne aykırı davranmış olması nedeniyle kusurlu olduğu değerlendirilebilir.</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>C kişisi ödeme yapmayı unutarak marketten çıkmıştır.</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.7170258760452271</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>C'nin dikkat ve özen yükümlülüğüne aykırı davranmış olması nedeniyle kusurlu olduğu değerlendirilebilir.</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>C kişisi hırsızdır ve hırsızlık suçu işlediği için bu durudman şüphe bile edilemez.</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.6190453767776489</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>C'nin dikkat ve özen yükümlülüğüne aykırı davranmış olması nedeniyle kusurlu olduğu değerlendirilebilir.</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>C kişisi bir banka müdürü.</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.5735637545585632</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>C'nin dikkat ve özen yükümlülüğüne aykırı davranmış olması nedeniyle kusurlu olduğu değerlendirilebilir.</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>C kişisinin mesleği banka müdürlüğüdür.</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.8778255581855774</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>C'nin dikkat ve özen yükümlülüğüne aykırı davranmış olması nedeniyle kusurlu olduğu değerlendirilebilir.</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>C'nin dikkat ve özen yükümlülüğüne aykırı davranmış olması nedeniyle kusurlu olduğu değerlendrilemez.</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>ENTAILMENT</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.7691475749015808</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>C'nin dikkat ve özen yükümlülüğüne aykırı davranmış olması nedeniyle kusurlu olduğu değerlendirilebilir.</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Leclerc, 2021 Formula 1 sezonunda 3. sırayı aldı.</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.5949161052703857</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>C'nin dikkat ve özen yükümlülüğüne aykırı davranmış olması nedeniyle kusurlu olduğu değerlendirilebilir.</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>C kişisi ödeme yapmadı sonra da marketten çıkarken ödemeyi unuttu.</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0.6229683756828308</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>C'nin dikkat ve özen yükümlülüğüne aykırı davranmış olması nedeniyle kusurlu olduğu değerlendirilebilir.</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>C kişisi kötü bir insan.</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0.6391960978507996</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>C'nin dikkat ve özen yükümlülüğüne aykırı davranmış olması nedeniyle kusurlu olduğu değerlendirilebilir.</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Kusurlu olan C kişisi, ödeme yapmayı unuttuğunu iddia etmektedir.</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0.3982060551643372</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>C'nin dikkat ve özen yükümlülüğüne aykırı davranmış olması nedeniyle kusurlu olduğu değerlendirilebilir.</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>C kişisi marketten çıkarken ödeme yapmayı unutmuştur.</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0.6342589259147644</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>C'nin dikkat ve özen yükümlülüğüne aykırı davranmış olması nedeniyle kusurlu olduğu değerlendrilemez.</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>C'nin dikkat ve özen yükümlülüğüne aykırı davranmış olması nedeniyle kusurlu olduğu değerlendirilebilir.</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>ENTAILMENT</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0.9611104726791382</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>C'nin dikkat ve özen yükümlülüğüne aykırı davranmış olması nedeniyle kusurlu olduğu değerlendrilemez.</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>C kişisi marketten alışveriş yapmıştır ve kasada ödeme yapmadan çıkmıştır.</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>0.5884826183319092</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>C'nin dikkat ve özen yükümlülüğüne aykırı davranmış olması nedeniyle kusurlu olduğu değerlendrilemez.</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>C kişisi ödeme yapmayı unutarak marketten çıkmıştır.</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0.7345539331436157</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>C'nin dikkat ve özen yükümlülüğüne aykırı davranmış olması nedeniyle kusurlu olduğu değerlendrilemez.</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>C kişisi hırsızdır ve hırsızlık suçu işlediği için bu durudman şüphe bile edilemez.</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>0.564023494720459</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>C'nin dikkat ve özen yükümlülüğüne aykırı davranmış olması nedeniyle kusurlu olduğu değerlendrilemez.</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>C kişisi bir banka müdürü.</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>0.5176191329956055</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>C'nin dikkat ve özen yükümlülüğüne aykırı davranmış olması nedeniyle kusurlu olduğu değerlendrilemez.</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>C kişisinin mesleği banka müdürlüğüdür.</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>0.8998844027519226</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>C'nin dikkat ve özen yükümlülüğüne aykırı davranmış olması nedeniyle kusurlu olduğu değerlendrilemez.</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>C'nin dikkat ve özen yükümlülüğüne aykırı davranmış olması nedeniyle kusurlu olduğu değerlendrilemez.</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>ENTAILMENT</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>0.9861453771591187</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>C'nin dikkat ve özen yükümlülüğüne aykırı davranmış olması nedeniyle kusurlu olduğu değerlendrilemez.</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Leclerc, 2021 Formula 1 sezonunda 3. sırayı aldı.</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>0.6025750637054443</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>C'nin dikkat ve özen yükümlülüğüne aykırı davranmış olması nedeniyle kusurlu olduğu değerlendrilemez.</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>C kişisi ödeme yapmadı sonra da marketten çıkarken ödemeyi unuttu.</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>0.6486769318580627</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>C'nin dikkat ve özen yükümlülüğüne aykırı davranmış olması nedeniyle kusurlu olduğu değerlendrilemez.</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>C kişisi kötü bir insan.</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>0.6597620844841003</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>C'nin dikkat ve özen yükümlülüğüne aykırı davranmış olması nedeniyle kusurlu olduğu değerlendrilemez.</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Kusurlu olan C kişisi, ödeme yapmayı unuttuğunu iddia etmektedir.</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>ENTAILMENT</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>0.4040274322032928</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>C'nin dikkat ve özen yükümlülüğüne aykırı davranmış olması nedeniyle kusurlu olduğu değerlendrilemez.</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>C kişisi marketten çıkarken ödeme yapmayı unutmuştur.</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>0.6388704180717468</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>C kişisi marketten alışveriş yapmıştır ve kasada ödeme yapmadan çıkmıştır.</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>C'nin dikkat ve özen yükümlülüğüne aykırı davranmış olması nedeniyle kusurlu olduğu değerlendirilebilir.</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>0.5278008580207825</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>C kişisi marketten alışveriş yapmıştır ve kasada ödeme yapmadan çıkmıştır.</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>C'nin dikkat ve özen yükümlülüğüne aykırı davranmış olması nedeniyle kusurlu olduğu değerlendrilemez.</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>0.6118601560592651</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>C kişisi marketten alışveriş yapmıştır ve kasada ödeme yapmadan çıkmıştır.</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>C kişisi ödeme yapmayı unutarak marketten çıkmıştır.</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>0.7739003896713257</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>C kişisi marketten alışveriş yapmıştır ve kasada ödeme yapmadan çıkmıştır.</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>C kişisi hırsızdır ve hırsızlık suçu işlediği için bu durudman şüphe bile edilemez.</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>0.4973465502262115</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>C kişisi marketten alışveriş yapmıştır ve kasada ödeme yapmadan çıkmıştır.</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>C kişisi bir banka müdürü.</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>0.8472043871879578</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>C kişisi marketten alışveriş yapmıştır ve kasada ödeme yapmadan çıkmıştır.</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>C kişisinin mesleği banka müdürlüğüdür.</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>0.9587122797966003</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>C kişisi marketten alışveriş yapmıştır ve kasada ödeme yapmadan çıkmıştır.</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>C'nin dikkat ve özen yükümlülüğüne aykırı davranmış olması nedeniyle kusurlu olduğu değerlendrilemez.</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>0.6118601560592651</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>C kişisi marketten alışveriş yapmıştır ve kasada ödeme yapmadan çıkmıştır.</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Leclerc, 2021 Formula 1 sezonunda 3. sırayı aldı.</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>0.6673837900161743</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>C kişisi marketten alışveriş yapmıştır ve kasada ödeme yapmadan çıkmıştır.</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>C kişisi ödeme yapmadı sonra da marketten çıkarken ödemeyi unuttu.</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>0.5868286490440369</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>C kişisi marketten alışveriş yapmıştır ve kasada ödeme yapmadan çıkmıştır.</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>C kişisi kötü bir insan.</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>0.7412387132644653</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>C kişisi marketten alışveriş yapmıştır ve kasada ödeme yapmadan çıkmıştır.</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Kusurlu olan C kişisi, ödeme yapmayı unuttuğunu iddia etmektedir.</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>0.6975939273834229</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>C kişisi marketten alışveriş yapmıştır ve kasada ödeme yapmadan çıkmıştır.</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>C kişisi marketten çıkarken ödeme yapmayı unutmuştur.</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>0.7404382228851318</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>C kişisi ödeme yapmayı unutarak marketten çıkmıştır.</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>C'nin dikkat ve özen yükümlülüğüne aykırı davranmış olması nedeniyle kusurlu olduğu değerlendirilebilir.</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>0.517585277557373</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>C kişisi ödeme yapmayı unutarak marketten çıkmıştır.</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>C'nin dikkat ve özen yükümlülüğüne aykırı davranmış olması nedeniyle kusurlu olduğu değerlendrilemez.</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>0.4837231040000916</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>C kişisi ödeme yapmayı unutarak marketten çıkmıştır.</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>C kişisi marketten alışveriş yapmıştır ve kasada ödeme yapmadan çıkmıştır.</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>0.7809376120567322</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>C kişisi ödeme yapmayı unutarak marketten çıkmıştır.</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>C kişisi hırsızdır ve hırsızlık suçu işlediği için bu durudman şüphe bile edilemez.</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>0.7549084424972534</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>C kişisi ödeme yapmayı unutarak marketten çıkmıştır.</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>C kişisi bir banka müdürü.</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>0.896523654460907</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>C kişisi ödeme yapmayı unutarak marketten çıkmıştır.</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>C kişisinin mesleği banka müdürlüğüdür.</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>0.932831883430481</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>C kişisi ödeme yapmayı unutarak marketten çıkmıştır.</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>C'nin dikkat ve özen yükümlülüğüne aykırı davranmış olması nedeniyle kusurlu olduğu değerlendrilemez.</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>0.4837231040000916</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>C kişisi ödeme yapmayı unutarak marketten çıkmıştır.</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Leclerc, 2021 Formula 1 sezonunda 3. sırayı aldı.</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>0.6630845069885254</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>C kişisi ödeme yapmayı unutarak marketten çıkmıştır.</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>C kişisi ödeme yapmadı sonra da marketten çıkarken ödemeyi unuttu.</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>ENTAILMENT</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>0.4828440546989441</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>C kişisi ödeme yapmayı unutarak marketten çıkmıştır.</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>C kişisi kötü bir insan.</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>0.8870726823806763</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>C kişisi ödeme yapmayı unutarak marketten çıkmıştır.</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Kusurlu olan C kişisi, ödeme yapmayı unuttuğunu iddia etmektedir.</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>0.4430281519889832</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>C kişisi ödeme yapmayı unutarak marketten çıkmıştır.</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>C kişisi marketten çıkarken ödeme yapmayı unutmuştur.</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>ENTAILMENT</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>0.9105066657066345</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>C kişisi hırsızdır ve hırsızlık suçu işlediği için bu durudman şüphe bile edilemez.</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>C'nin dikkat ve özen yükümlülüğüne aykırı davranmış olması nedeniyle kusurlu olduğu değerlendirilebilir.</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>0.4570322632789612</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>C kişisi hırsızdır ve hırsızlık suçu işlediği için bu durudman şüphe bile edilemez.</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>C'nin dikkat ve özen yükümlülüğüne aykırı davranmış olması nedeniyle kusurlu olduğu değerlendrilemez.</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>0.5596138834953308</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>C kişisi hırsızdır ve hırsızlık suçu işlediği için bu durudman şüphe bile edilemez.</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>C kişisi marketten alışveriş yapmıştır ve kasada ödeme yapmadan çıkmıştır.</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>0.6220995187759399</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>C kişisi hırsızdır ve hırsızlık suçu işlediği için bu durudman şüphe bile edilemez.</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>C kişisi ödeme yapmayı unutarak marketten çıkmıştır.</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>0.6555491089820862</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>C kişisi hırsızdır ve hırsızlık suçu işlediği için bu durudman şüphe bile edilemez.</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>C kişisi bir banka müdürü.</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>0.5217778086662292</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>C kişisi hırsızdır ve hırsızlık suçu işlediği için bu durudman şüphe bile edilemez.</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>C kişisinin mesleği banka müdürlüğüdür.</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>0.6414043307304382</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>C kişisi hırsızdır ve hırsızlık suçu işlediği için bu durudman şüphe bile edilemez.</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>C'nin dikkat ve özen yükümlülüğüne aykırı davranmış olması nedeniyle kusurlu olduğu değerlendrilemez.</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>0.5596138834953308</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>C kişisi hırsızdır ve hırsızlık suçu işlediği için bu durudman şüphe bile edilemez.</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Leclerc, 2021 Formula 1 sezonunda 3. sırayı aldı.</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>0.6893278956413269</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>C kişisi hırsızdır ve hırsızlık suçu işlediği için bu durudman şüphe bile edilemez.</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>C kişisi ödeme yapmadı sonra da marketten çıkarken ödemeyi unuttu.</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>0.7910680174827576</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>C kişisi hırsızdır ve hırsızlık suçu işlediği için bu durudman şüphe bile edilemez.</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>C kişisi kötü bir insan.</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>0.8199467062950134</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>C kişisi hırsızdır ve hırsızlık suçu işlediği için bu durudman şüphe bile edilemez.</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Kusurlu olan C kişisi, ödeme yapmayı unuttuğunu iddia etmektedir.</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>0.8159048557281494</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>C kişisi hırsızdır ve hırsızlık suçu işlediği için bu durudman şüphe bile edilemez.</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>C kişisi marketten çıkarken ödeme yapmayı unutmuştur.</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>0.7553998827934265</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>C kişisi bir banka müdürü.</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>C'nin dikkat ve özen yükümlülüğüne aykırı davranmış olması nedeniyle kusurlu olduğu değerlendirilebilir.</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>0.7721019387245178</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>C kişisi bir banka müdürü.</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>C'nin dikkat ve özen yükümlülüğüne aykırı davranmış olması nedeniyle kusurlu olduğu değerlendrilemez.</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>0.7254020571708679</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>C kişisi bir banka müdürü.</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>C kişisi marketten alışveriş yapmıştır ve kasada ödeme yapmadan çıkmıştır.</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>0.6083983778953552</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>C kişisi bir banka müdürü.</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>C kişisi ödeme yapmayı unutarak marketten çıkmıştır.</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>0.89566570520401</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>C kişisi bir banka müdürü.</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>C kişisi hırsızdır ve hırsızlık suçu işlediği için bu durudman şüphe bile edilemez.</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>0.8339878916740417</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>C kişisi bir banka müdürü.</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>C kişisinin mesleği banka müdürlüğüdür.</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>0.7127555012702942</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>C kişisi bir banka müdürü.</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>C'nin dikkat ve özen yükümlülüğüne aykırı davranmış olması nedeniyle kusurlu olduğu değerlendrilemez.</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>0.7254020571708679</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>C kişisi bir banka müdürü.</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Leclerc, 2021 Formula 1 sezonunda 3. sırayı aldı.</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>0.7167258262634277</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>C kişisi bir banka müdürü.</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>C kişisi ödeme yapmadı sonra da marketten çıkarken ödemeyi unuttu.</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>0.8262656331062317</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>C kişisi bir banka müdürü.</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>C kişisi kötü bir insan.</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>0.8895009756088257</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>C kişisi bir banka müdürü.</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Kusurlu olan C kişisi, ödeme yapmayı unuttuğunu iddia etmektedir.</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>0.5186174511909485</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>C kişisi bir banka müdürü.</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>C kişisi marketten çıkarken ödeme yapmayı unutmuştur.</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>0.8955378532409668</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>C kişisinin mesleği banka müdürlüğüdür.</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>C'nin dikkat ve özen yükümlülüğüne aykırı davranmış olması nedeniyle kusurlu olduğu değerlendirilebilir.</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>0.5781448483467102</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>C kişisinin mesleği banka müdürlüğüdür.</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>C'nin dikkat ve özen yükümlülüğüne aykırı davranmış olması nedeniyle kusurlu olduğu değerlendrilemez.</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>0.5470118522644043</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>C kişisinin mesleği banka müdürlüğüdür.</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>C kişisi marketten alışveriş yapmıştır ve kasada ödeme yapmadan çıkmıştır.</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>0.5039349794387817</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>C kişisinin mesleği banka müdürlüğüdür.</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>C kişisi ödeme yapmayı unutarak marketten çıkmıştır.</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>CONTRADICTION</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>0.8684171438217163</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>